<commit_message>
Added sticky registration, social media
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>s</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>admin page</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>lalabas lang sa search pag wala pang naaadd</t>
   </si>
 </sst>
 </file>
@@ -587,7 +593,7 @@
   <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +717,9 @@
       <c r="G6" t="s">
         <v>35</v>
       </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
       <c r="J6" t="s">
         <v>65</v>
       </c>
@@ -803,6 +812,9 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -813,6 +825,9 @@
       </c>
       <c r="D14" t="s">
         <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Company Completion Form
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -4,22 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245"/>
   </bookViews>
   <sheets>
-    <sheet name="FLOW" sheetId="1" r:id="rId1"/>
-    <sheet name="db" sheetId="2" r:id="rId2"/>
-    <sheet name="design" sheetId="3" r:id="rId3"/>
+    <sheet name="db" sheetId="2" r:id="rId1"/>
+    <sheet name="design" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
-  <si>
-    <t>s</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>db_user</t>
   </si>
@@ -573,30 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,295 +584,295 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -905,19 +881,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Employer signup, added job posting, viewing, employers profile
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>db_user</t>
   </si>
@@ -119,12 +119,6 @@
     <t>desc</t>
   </si>
   <si>
-    <t>recruiter_email</t>
-  </si>
-  <si>
-    <t>recruiter_id</t>
-  </si>
-  <si>
     <t>processing_time</t>
   </si>
   <si>
@@ -222,6 +216,12 @@
   </si>
   <si>
     <t>https://htmlstream.com/preview/front-v1.2/html/home/index.html</t>
+  </si>
+  <si>
+    <t>expire_date</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -245,12 +245,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -265,9 +277,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,56 +586,62 @@
   <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="31.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -634,17 +654,17 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
@@ -654,20 +674,20 @@
         <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
@@ -677,202 +697,205 @@
         <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>60</v>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>61</v>
+      <c r="D11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" t="s">
-        <v>46</v>
+      <c r="F15" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>46</v>
+      <c r="D18" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>59</v>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>44</v>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>45</v>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>56</v>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>57</v>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -885,15 +908,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added applicant's employment history
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>db_user</t>
   </si>
@@ -222,6 +222,48 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>add location</t>
+  </si>
+  <si>
+    <t>add required skills</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>startdate</t>
+  </si>
+  <si>
+    <t>end date</t>
+  </si>
+  <si>
+    <t>job role</t>
+  </si>
+  <si>
+    <t>db_education</t>
+  </si>
+  <si>
+    <t>check github profile design</t>
+  </si>
+  <si>
+    <t>add cover letter</t>
+  </si>
+  <si>
+    <t>brief desc about self</t>
+  </si>
+  <si>
+    <t>allow to link to existing company</t>
+  </si>
+  <si>
+    <t>job description</t>
+  </si>
+  <si>
+    <t>companyid(if linked)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +306,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -277,11 +325,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,318 +632,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J24"/>
+  <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="31.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="29.7109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="I16" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="s">
+      <c r="I17" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="2" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -906,9 +1005,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -917,6 +1018,11 @@
         <v>66</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added change pw, slideshow, notifications,admin settings
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>db_user</t>
   </si>
@@ -271,6 +271,30 @@
   </si>
   <si>
     <t>add skills ratings to job post</t>
+  </si>
+  <si>
+    <t>homepage</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>applicant email</t>
+  </si>
+  <si>
+    <t>edit company</t>
+  </si>
+  <si>
+    <t>feather</t>
+  </si>
+  <si>
+    <t>turn off error reporting</t>
+  </si>
+  <si>
+    <t>restrict access</t>
+  </si>
+  <si>
+    <t>change pw</t>
   </si>
 </sst>
 </file>
@@ -641,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1037,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,6 +1079,46 @@
         <v>84</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>